<commit_message>
Eventuele missende bestanden commit
</commit_message>
<xml_diff>
--- a/TimeTable.xlsx
+++ b/TimeTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>week 1</t>
   </si>
@@ -278,9 +278,6 @@
   </si>
   <si>
     <t>3D meshes Weapons</t>
-  </si>
-  <si>
-    <t>Kruipen</t>
   </si>
 </sst>
 </file>
@@ -326,7 +323,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,14 +354,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -424,46 +415,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -486,6 +442,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,13 +470,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -507,16 +481,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -526,45 +500,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -852,18 +787,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P37"/>
+  <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" style="30" customWidth="1"/>
-    <col min="4" max="5" width="19.77734375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="19.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="19.77734375" style="1" customWidth="1"/>
     <col min="9" max="10" width="19.77734375" style="2" customWidth="1"/>
@@ -871,138 +805,130 @@
     <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="2:12" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="21"/>
-    </row>
-    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="28"/>
-    </row>
-    <row r="3" spans="2:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="29" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
+    </row>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="26"/>
-    </row>
-    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="27"/>
-    </row>
-    <row r="5" spans="2:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="16" t="s">
+    </row>
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="2:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="2:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="12" t="s">
+    </row>
+    <row r="9" spans="2:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="2:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="2:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E14" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F16" s="16" t="s">
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="3:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E17" s="3" t="s">
@@ -1047,20 +973,20 @@
       </c>
     </row>
     <row r="20" spans="3:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
       <c r="E21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="21" t="s">
         <v>31</v>
       </c>
       <c r="H21" s="2"/>
@@ -1069,10 +995,10 @@
       <c r="E22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="21" t="s">
         <v>31</v>
       </c>
       <c r="H22" s="2"/>
@@ -1083,10 +1009,10 @@
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="I24" s="15" t="s">
+      <c r="I24" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="15"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
       <c r="I25" s="7" t="s">
@@ -1103,17 +1029,17 @@
     <row r="27" spans="3:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="3:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="23" t="s">
         <v>56</v>
       </c>
       <c r="K29" s="6" t="s">
@@ -1121,12 +1047,12 @@
       </c>
     </row>
     <row r="30" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="24" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="3:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L31" s="9" t="s">
+      <c r="L31" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1137,7 +1063,7 @@
       </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1169,7 +1095,7 @@
       </c>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="1" t="s">

</xml_diff>